<commit_message>
more attribute scripts, texts for categories and attributes
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C0D2947-EC99-4744-9B33-8FDF576AFF42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC6FB9C-9A3D-4D52-8743-92D7070873BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="1290" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1980" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Key</t>
   </si>
@@ -110,6 +110,216 @@
   </si>
   <si>
     <t>Kero Shapes</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>property</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>triangle</t>
+  </si>
+  <si>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>quadrilateral</t>
+  </si>
+  <si>
+    <t>Quadrilateral</t>
+  </si>
+  <si>
+    <t>pentagon</t>
+  </si>
+  <si>
+    <t>Pentagon</t>
+  </si>
+  <si>
+    <t>hexagon</t>
+  </si>
+  <si>
+    <t>Hexagon</t>
+  </si>
+  <si>
+    <t>polygon</t>
+  </si>
+  <si>
+    <t>Polygon</t>
+  </si>
+  <si>
+    <t>triangle_right</t>
+  </si>
+  <si>
+    <t>Right Triangle</t>
+  </si>
+  <si>
+    <t>triangle_equilateral</t>
+  </si>
+  <si>
+    <t>Equilateral Triangle</t>
+  </si>
+  <si>
+    <t>triangle_isosceles</t>
+  </si>
+  <si>
+    <t>Isosceles Triangle</t>
+  </si>
+  <si>
+    <t>triangle_scalene</t>
+  </si>
+  <si>
+    <t>Scalene Triangle</t>
+  </si>
+  <si>
+    <t>triangle_acute</t>
+  </si>
+  <si>
+    <t>Acute Triangle</t>
+  </si>
+  <si>
+    <t>triangle_obtuse</t>
+  </si>
+  <si>
+    <t>Obtuse Triangle</t>
+  </si>
+  <si>
+    <t>quad_rectangle</t>
+  </si>
+  <si>
+    <t>Rectangle</t>
+  </si>
+  <si>
+    <t>quad_square</t>
+  </si>
+  <si>
+    <t>Square</t>
+  </si>
+  <si>
+    <t>quad_rhombus</t>
+  </si>
+  <si>
+    <t>Rhombus</t>
+  </si>
+  <si>
+    <t>quad_parallelogram</t>
+  </si>
+  <si>
+    <t>Parallelogram</t>
+  </si>
+  <si>
+    <t>quad_trapezoid</t>
+  </si>
+  <si>
+    <t>Trapezoid</t>
+  </si>
+  <si>
+    <t>quad_trapezium</t>
+  </si>
+  <si>
+    <t>Trapezium</t>
+  </si>
+  <si>
+    <t>quad_kite</t>
+  </si>
+  <si>
+    <t>Kite</t>
+  </si>
+  <si>
+    <t>prop_90_degree</t>
+  </si>
+  <si>
+    <t>Has a 90° angle.</t>
+  </si>
+  <si>
+    <t>prop_sides_equal_all</t>
+  </si>
+  <si>
+    <t>prop_60_degree_all</t>
+  </si>
+  <si>
+    <t>All sides are equal.</t>
+  </si>
+  <si>
+    <t>prop_sides_equal_two</t>
+  </si>
+  <si>
+    <t>Two equal sides.</t>
+  </si>
+  <si>
+    <t>prop_angles_equal_two</t>
+  </si>
+  <si>
+    <t>Two equal angles.</t>
+  </si>
+  <si>
+    <t>No sides are equal.</t>
+  </si>
+  <si>
+    <t>prop_sides_no_equal</t>
+  </si>
+  <si>
+    <t>prop_angles_less_90_all</t>
+  </si>
+  <si>
+    <t>All angles &lt; 90°.</t>
+  </si>
+  <si>
+    <t>All angles = 60°.</t>
+  </si>
+  <si>
+    <t>prop_angle_greater_90</t>
+  </si>
+  <si>
+    <t>Has an angle &gt; 90°.</t>
+  </si>
+  <si>
+    <t>prop_90_degree_all</t>
+  </si>
+  <si>
+    <t>All angles = 90°.</t>
+  </si>
+  <si>
+    <t>prop_opposite_sides_parallel</t>
+  </si>
+  <si>
+    <t>Opposite sides are parallel.</t>
+  </si>
+  <si>
+    <t>prop_opposite_sides_equal</t>
+  </si>
+  <si>
+    <t>Opposite sides are equal.</t>
+  </si>
+  <si>
+    <t>prop_opposite_angles_equal</t>
+  </si>
+  <si>
+    <t>Opposite angles are equal.</t>
+  </si>
+  <si>
+    <t>prop_opposite_pair_parallel</t>
+  </si>
+  <si>
+    <t>Two sides are parallel.</t>
+  </si>
+  <si>
+    <t>prop_sides_no_parallel</t>
+  </si>
+  <si>
+    <t>No sides are parallel.</t>
+  </si>
+  <si>
+    <t>Two pairs of sides are equal.</t>
+  </si>
+  <si>
+    <t>prop_sides_pair_equal</t>
   </si>
 </sst>
 </file>
@@ -445,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,6 +793,382 @@
         <v>20</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>80</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
some tweaks, added categories and attributes data
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBC6FB9C-9A3D-4D52-8743-92D7070873BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93223057-CE5D-4A2E-A0CE-6B651CA89105}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1905" yWindow="1980" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>Key</t>
   </si>
@@ -320,6 +320,54 @@
   </si>
   <si>
     <t>prop_sides_pair_equal</t>
+  </si>
+  <si>
+    <t>octagon</t>
+  </si>
+  <si>
+    <t>Octagon</t>
+  </si>
+  <si>
+    <t>decagon</t>
+  </si>
+  <si>
+    <t>Decagon</t>
+  </si>
+  <si>
+    <t>prop_side_3</t>
+  </si>
+  <si>
+    <t>prop_side_4</t>
+  </si>
+  <si>
+    <t>prop_side_5</t>
+  </si>
+  <si>
+    <t>prop_side_6</t>
+  </si>
+  <si>
+    <t>prop_side_8</t>
+  </si>
+  <si>
+    <t>prop_side_10</t>
+  </si>
+  <si>
+    <t>Has 3 sides.</t>
+  </si>
+  <si>
+    <t>Has 5 sides.</t>
+  </si>
+  <si>
+    <t>Has 6 sides.</t>
+  </si>
+  <si>
+    <t>Has 8 sides.</t>
+  </si>
+  <si>
+    <t>Has 10 sides.</t>
+  </si>
+  <si>
+    <t>Has 4 sides.</t>
   </si>
 </sst>
 </file>
@@ -655,10 +703,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,32 +911,32 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>45</v>
+        <v>101</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>47</v>
+        <v>103</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -896,10 +944,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -907,10 +955,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -918,10 +966,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -929,10 +977,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -940,10 +988,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -951,10 +999,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -962,142 +1010,142 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C32">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C33">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>76</v>
+        <v>115</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>81</v>
+        <v>108</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>85</v>
+        <v>114</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="C43">
         <v>3</v>
@@ -1105,10 +1153,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="C44">
         <v>3</v>
@@ -1116,10 +1164,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C45">
         <v>3</v>
@@ -1127,10 +1175,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="C46">
         <v>3</v>
@@ -1138,10 +1186,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="C47">
         <v>3</v>
@@ -1149,10 +1197,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C48">
         <v>3</v>
@@ -1160,12 +1208,100 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>94</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>96</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C49">
+      <c r="C57">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
spaceship stuff, initial shape category ui
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93223057-CE5D-4A2E-A0CE-6B651CA89105}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35C096A-B85E-457E-B4AF-3021AA626B20}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1980" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5250" yWindow="2205" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>Key</t>
   </si>
@@ -368,6 +368,12 @@
   </si>
   <si>
     <t>Has 4 sides.</t>
+  </si>
+  <si>
+    <t>shape_categories</t>
+  </si>
+  <si>
+    <t>Shape Categories</t>
   </si>
 </sst>
 </file>
@@ -703,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,6 +1311,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
shape analyzer setup, shape category implement
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35C096A-B85E-457E-B4AF-3021AA626B20}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BC0B72-E7A8-4A84-A30F-D8490DFA3B4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5250" yWindow="2205" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>Key</t>
   </si>
@@ -268,24 +268,12 @@
     <t>prop_angles_less_90_all</t>
   </si>
   <si>
-    <t>All angles &lt; 90°.</t>
-  </si>
-  <si>
-    <t>All angles = 60°.</t>
-  </si>
-  <si>
     <t>prop_angle_greater_90</t>
   </si>
   <si>
-    <t>Has an angle &gt; 90°.</t>
-  </si>
-  <si>
     <t>prop_90_degree_all</t>
   </si>
   <si>
-    <t>All angles = 90°.</t>
-  </si>
-  <si>
     <t>prop_opposite_sides_parallel</t>
   </si>
   <si>
@@ -352,28 +340,64 @@
     <t>prop_side_10</t>
   </si>
   <si>
-    <t>Has 3 sides.</t>
-  </si>
-  <si>
-    <t>Has 5 sides.</t>
-  </si>
-  <si>
-    <t>Has 6 sides.</t>
-  </si>
-  <si>
-    <t>Has 8 sides.</t>
-  </si>
-  <si>
-    <t>Has 10 sides.</t>
-  </si>
-  <si>
-    <t>Has 4 sides.</t>
-  </si>
-  <si>
     <t>shape_categories</t>
   </si>
   <si>
     <t>Shape Categories</t>
+  </si>
+  <si>
+    <t>proceed_instruct</t>
+  </si>
+  <si>
+    <t>Press this button to proceed.</t>
+  </si>
+  <si>
+    <t>3 sides.</t>
+  </si>
+  <si>
+    <t>4 sides.</t>
+  </si>
+  <si>
+    <t>5 sides.</t>
+  </si>
+  <si>
+    <t>6 sides.</t>
+  </si>
+  <si>
+    <t>8 sides.</t>
+  </si>
+  <si>
+    <t>10 sides.</t>
+  </si>
+  <si>
+    <t>All angles equal 60°.</t>
+  </si>
+  <si>
+    <t>All angles equal 90°.</t>
+  </si>
+  <si>
+    <t>Has an angle greater than 90°.</t>
+  </si>
+  <si>
+    <t>All angles less than 90°.</t>
+  </si>
+  <si>
+    <t>categories_title</t>
+  </si>
+  <si>
+    <t>CATEGORIES</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>rank</t>
+  </si>
+  <si>
+    <t>Rank:</t>
+  </si>
+  <si>
+    <t>Score:</t>
   </si>
 </sst>
 </file>
@@ -709,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,59 +881,50 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>33</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>123</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18">
-        <v>1.5</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19">
-        <v>1.5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20">
-        <v>1.5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C21">
         <v>1.5</v>
@@ -917,10 +932,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>100</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="C22">
         <v>1.5</v>
@@ -928,10 +943,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -939,43 +954,43 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>47</v>
+        <v>97</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>49</v>
+        <v>99</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -983,10 +998,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -994,10 +1009,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1005,10 +1020,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -1016,10 +1031,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1027,10 +1042,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -1038,87 +1053,87 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C34">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C35">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>115</v>
+        <v>67</v>
       </c>
       <c r="C38">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>111</v>
+        <v>69</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -1126,10 +1141,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -1137,10 +1152,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -1148,43 +1163,43 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>103</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
       <c r="C44">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>105</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C46">
         <v>3</v>
@@ -1192,10 +1207,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C47">
         <v>3</v>
@@ -1203,10 +1218,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C48">
         <v>3</v>
@@ -1214,10 +1229,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C49">
         <v>3</v>
@@ -1225,10 +1240,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -1236,10 +1251,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -1247,10 +1262,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C52">
         <v>3</v>
@@ -1258,10 +1273,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="C53">
         <v>3</v>
@@ -1269,10 +1284,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="C54">
         <v>3</v>
@@ -1280,10 +1295,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C55">
         <v>3</v>
@@ -1291,10 +1306,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -1302,10 +1317,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C57">
         <v>3</v>
@@ -1313,10 +1328,54 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>117</v>
+        <v>91</v>
+      </c>
+      <c r="C58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>108</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
collect counter, victory, game flow
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BC0B72-E7A8-4A84-A30F-D8490DFA3B4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7D7D97-8D74-4BDE-864E-EF7C7663E70D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5250" yWindow="2205" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
   <si>
     <t>Key</t>
   </si>
@@ -398,6 +398,18 @@
   </si>
   <si>
     <t>Score:</t>
+  </si>
+  <si>
+    <t>victory</t>
+  </si>
+  <si>
+    <t>VICTORY</t>
+  </si>
+  <si>
+    <t>score_total</t>
+  </si>
+  <si>
+    <t>Total Score:</t>
   </si>
 </sst>
 </file>
@@ -733,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,45 +909,42 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21">
-        <v>1.5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22">
         <v>1.5</v>
@@ -943,10 +952,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C23">
         <v>1.5</v>
@@ -954,10 +963,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -965,10 +974,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>40</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>97</v>
+        <v>41</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -976,10 +985,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C26">
         <v>1.5</v>
@@ -987,21 +996,21 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1009,10 +1018,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -1020,10 +1029,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -1031,10 +1040,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1042,10 +1051,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -1053,10 +1062,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -1064,10 +1073,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -1075,10 +1084,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -1086,32 +1095,32 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C37">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C38">
         <v>2.5</v>
@@ -1119,32 +1128,32 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -1152,10 +1161,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -1163,10 +1172,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -1174,10 +1183,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -1185,10 +1194,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -1196,21 +1205,21 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>105</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="C46">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C47">
         <v>3</v>
@@ -1218,10 +1227,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="C48">
         <v>3</v>
@@ -1229,10 +1238,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>76</v>
+        <v>116</v>
       </c>
       <c r="C49">
         <v>3</v>
@@ -1240,10 +1249,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -1251,10 +1260,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -1262,10 +1271,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>119</v>
+        <v>79</v>
       </c>
       <c r="C52">
         <v>3</v>
@@ -1273,10 +1282,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C53">
         <v>3</v>
@@ -1284,10 +1293,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C54">
         <v>3</v>
@@ -1295,10 +1304,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
       <c r="C55">
         <v>3</v>
@@ -1306,10 +1315,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -1317,10 +1326,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C57">
         <v>3</v>
@@ -1328,10 +1337,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C58">
         <v>3</v>
@@ -1339,10 +1348,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C59">
         <v>3</v>
@@ -1350,10 +1359,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C60">
         <v>3</v>
@@ -1361,21 +1370,40 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>107</v>
+        <v>94</v>
+      </c>
+      <c r="C61">
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>108</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C62">
-        <v>3</v>
+      <c r="C63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
victory animation, level 0-2
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7D7D97-8D74-4BDE-864E-EF7C7663E70D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C7458D-8A99-401C-B8EE-D7CFD38453CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5250" yWindow="2205" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5985" yWindow="2745" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t>Key</t>
   </si>
@@ -410,6 +410,120 @@
   </si>
   <si>
     <t>Total Score:</t>
+  </si>
+  <si>
+    <t>shapes</t>
+  </si>
+  <si>
+    <t>Shapes</t>
+  </si>
+  <si>
+    <t>ellipse</t>
+  </si>
+  <si>
+    <t>Ellipse</t>
+  </si>
+  <si>
+    <t>blob</t>
+  </si>
+  <si>
+    <t>Blob</t>
+  </si>
+  <si>
+    <t>ellipse_desc</t>
+  </si>
+  <si>
+    <t>blob_desc</t>
+  </si>
+  <si>
+    <t>poly_desc</t>
+  </si>
+  <si>
+    <t>· Has a center point.\n\n· Dimensions defined by two axis.</t>
+  </si>
+  <si>
+    <t>side</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>Point (x, y)</t>
+  </si>
+  <si>
+    <t>Side (length)</t>
+  </si>
+  <si>
+    <t>Welcome to Kero Shapes!</t>
+  </si>
+  <si>
+    <t>intro_0_0</t>
+  </si>
+  <si>
+    <t>intro_0_1</t>
+  </si>
+  <si>
+    <t>intro_0_2</t>
+  </si>
+  <si>
+    <t>When it comes to categorizing shapes, one must figure out the common attributes they share.</t>
+  </si>
+  <si>
+    <t>intro_1_0</t>
+  </si>
+  <si>
+    <t>intro_1_1</t>
+  </si>
+  <si>
+    <t>· Made up of curves defined by equations.</t>
+  </si>
+  <si>
+    <t>intro_2_0</t>
+  </si>
+  <si>
+    <t>For now, we will be focusing on identifying polygons.</t>
+  </si>
+  <si>
+    <t>intro_3_0</t>
+  </si>
+  <si>
+    <t>Now let's go forth, and help these lads survey the land!</t>
+  </si>
+  <si>
+    <t>In this game, you will be helping these fine capable frogs to categorize shapes that are scattered about in the land.</t>
+  </si>
+  <si>
+    <t>Here are some primary categories and their attributes that differentiate them from each other.</t>
+  </si>
+  <si>
+    <t>level_intro_0_0</t>
+  </si>
+  <si>
+    <t>instruct_collect</t>
+  </si>
+  <si>
+    <t>Press and hold the shape to collect it.</t>
+  </si>
+  <si>
+    <t>instruct_category_drag</t>
+  </si>
+  <si>
+    <t>Press and drag the item towards the category, and release.</t>
+  </si>
+  <si>
+    <t>The following types of shapes will come up. Be sure to remember them!</t>
+  </si>
+  <si>
+    <t>level_0_continue</t>
+  </si>
+  <si>
+    <t>Go ahead and collect the rest of the shapes! Remember to match them with the correct category.</t>
+  </si>
+  <si>
+    <t>· Has three or more points plotted on a plane.\n\n· Has a number of sides connected by points.</t>
+  </si>
+  <si>
+    <t>Remember that a polygon is formed by three or more straight lines that are connected in a loop.</t>
   </si>
 </sst>
 </file>
@@ -745,10 +859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,40 +1047,34 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>132</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>43</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>134</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22">
-        <v>1.5</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23">
-        <v>1.5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C24">
         <v>1.5</v>
@@ -974,10 +1082,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C25">
         <v>1.5</v>
@@ -985,10 +1093,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="C26">
         <v>1.5</v>
@@ -996,10 +1104,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="C27">
         <v>1.5</v>
@@ -1007,32 +1115,32 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -1040,10 +1148,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1051,10 +1159,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -1062,10 +1170,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -1073,10 +1181,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -1084,10 +1192,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -1095,10 +1203,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -1106,76 +1214,76 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C38">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C39">
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>110</v>
+        <v>67</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>111</v>
+        <v>69</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -1183,10 +1291,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -1194,10 +1302,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -1205,10 +1313,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -1216,32 +1324,32 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="C47">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>74</v>
+        <v>115</v>
       </c>
       <c r="C48">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="C49">
         <v>3</v>
@@ -1249,10 +1357,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -1260,10 +1368,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="C51">
         <v>3</v>
@@ -1271,10 +1379,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C52">
         <v>3</v>
@@ -1282,10 +1390,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="C53">
         <v>3</v>
@@ -1293,10 +1401,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="C54">
         <v>3</v>
@@ -1304,10 +1412,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C55">
         <v>3</v>
@@ -1315,10 +1423,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>85</v>
+        <v>118</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -1326,10 +1434,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>87</v>
+        <v>117</v>
       </c>
       <c r="C57">
         <v>3</v>
@@ -1337,10 +1445,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C58">
         <v>3</v>
@@ -1348,10 +1456,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C59">
         <v>3</v>
@@ -1359,10 +1467,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C60">
         <v>3</v>
@@ -1370,10 +1478,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C61">
         <v>3</v>
@@ -1381,18 +1489,21 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>107</v>
+        <v>93</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C63">
         <v>3</v>
@@ -1400,10 +1511,165 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>106</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>108</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>126</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>137</v>
+      </c>
+      <c r="B69" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>141</v>
+      </c>
+      <c r="B72" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>159</v>
+      </c>
+      <c r="B73" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>161</v>
+      </c>
+      <c r="B74" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>146</v>
+      </c>
+      <c r="B76" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>149</v>
+      </c>
+      <c r="B78" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>150</v>
+      </c>
+      <c r="B79" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>152</v>
+      </c>
+      <c r="B80" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>154</v>
+      </c>
+      <c r="B81" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>158</v>
+      </c>
+      <c r="B82" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some tweaks, levels 3-5
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C7458D-8A99-401C-B8EE-D7CFD38453CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5300B8-456C-4F5C-A97F-B18A7BC36F60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5985" yWindow="2745" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <si>
     <t>Key</t>
   </si>
@@ -439,9 +439,6 @@
     <t>poly_desc</t>
   </si>
   <si>
-    <t>· Has a center point.\n\n· Dimensions defined by two axis.</t>
-  </si>
-  <si>
     <t>side</t>
   </si>
   <si>
@@ -520,10 +517,55 @@
     <t>Go ahead and collect the rest of the shapes! Remember to match them with the correct category.</t>
   </si>
   <si>
-    <t>· Has three or more points plotted on a plane.\n\n· Has a number of sides connected by points.</t>
-  </si>
-  <si>
     <t>Remember that a polygon is formed by three or more straight lines that are connected in a loop.</t>
+  </si>
+  <si>
+    <t>· Round, has a center point.\n\n· Dimensions defined by two axis.</t>
+  </si>
+  <si>
+    <t>tri_desc</t>
+  </si>
+  <si>
+    <t>level_intro_3_0</t>
+  </si>
+  <si>
+    <t>level_intro_3_1</t>
+  </si>
+  <si>
+    <t>level_intro_3_2</t>
+  </si>
+  <si>
+    <t>level_intro_3_3</t>
+  </si>
+  <si>
+    <t>Now that we've covered some of the polygons, let's take a closer look at triangles.</t>
+  </si>
+  <si>
+    <t>For this level, we will be looking at different triangles based on their angle values. Be sure to remember them!</t>
+  </si>
+  <si>
+    <t>With that in mind, we can then further identify sub-categories under the triangle with additional attributes.</t>
+  </si>
+  <si>
+    <t>level_intro_4_0</t>
+  </si>
+  <si>
+    <t>· Formed by three or more straight lines (sides) connected in a loop.\n\n· Points are plotted on a plane.</t>
+  </si>
+  <si>
+    <t>· Formed by three straight lines connected in a loop.\n· Points are plotted on a plane.\n· Angles sum up to 180°.</t>
+  </si>
+  <si>
+    <t>As a sub-category of polygons, triangles follow the same attribute of being formed by a number of straight lines connected in a loop. In this case, there are three.</t>
+  </si>
+  <si>
+    <t>level_intro_5_0</t>
+  </si>
+  <si>
+    <t>Now that we've seen some triangles based on their angle values, let's take a look at the ones based on their side values.</t>
+  </si>
+  <si>
+    <t>For this level, we will be categorizing triangles based on their angles, and side lengths. These triangles will have more than one category that fit their attributes.</t>
   </si>
 </sst>
 </file>
@@ -859,10 +901,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,7 +1591,7 @@
         <v>136</v>
       </c>
       <c r="B68" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -1557,7 +1599,7 @@
         <v>137</v>
       </c>
       <c r="B69" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1565,20 +1607,20 @@
         <v>138</v>
       </c>
       <c r="B70" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B72" t="s">
         <v>142</v>
@@ -1586,90 +1628,146 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>159</v>
+        <v>140</v>
       </c>
       <c r="B73" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B74" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="B75" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B76" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B77" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B78" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B79" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>149</v>
+      </c>
+      <c r="B80" t="s">
         <v>152</v>
-      </c>
-      <c r="B80" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B82" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>157</v>
+      </c>
+      <c r="B83" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>163</v>
+      </c>
+      <c r="B84" t="s">
         <v>164</v>
       </c>
-      <c r="B83" t="s">
-        <v>165</v>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>169</v>
+      </c>
+      <c r="B86" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>170</v>
+      </c>
+      <c r="B87" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>171</v>
+      </c>
+      <c r="B88" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>179</v>
+      </c>
+      <c r="B90" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some level 6 stuff
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5300B8-456C-4F5C-A97F-B18A7BC36F60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DDBA74-3D89-4688-AA01-4CAA74E5E610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5985" yWindow="2745" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6075" yWindow="2475" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="192">
   <si>
     <t>Key</t>
   </si>
@@ -566,6 +566,36 @@
   </si>
   <si>
     <t>For this level, we will be categorizing triangles based on their angles, and side lengths. These triangles will have more than one category that fit their attributes.</t>
+  </si>
+  <si>
+    <t>quad_desc</t>
+  </si>
+  <si>
+    <t>· Formed by four straight lines connected in a loop.\n· Points are plotted on a plane.\n· Angles sum up to 360°.</t>
+  </si>
+  <si>
+    <t>level_intro_6_0</t>
+  </si>
+  <si>
+    <t>We'll now be looking at the next sub-category of polygons, the quadrilaterals.</t>
+  </si>
+  <si>
+    <t>level_intro_6_1</t>
+  </si>
+  <si>
+    <t>level_intro_6_2</t>
+  </si>
+  <si>
+    <t>level_intro_6_3</t>
+  </si>
+  <si>
+    <t>As the name suggests, it is four-sided.</t>
+  </si>
+  <si>
+    <t>For this level, we'll be looking at three particular sub-categories that all have two pairs of opposite, parallel, equal-length sides.</t>
+  </si>
+  <si>
+    <t>Just as certain triangles have more than one matching categories, so does quadrilaterals. Keep that in mind!</t>
   </si>
 </sst>
 </file>
@@ -901,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,154 +1650,194 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>182</v>
       </c>
       <c r="B72" t="s">
-        <v>142</v>
+        <v>183</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B73" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="B74" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B75" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="B76" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B77" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B78" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B79" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B80" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B81" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B82" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B83" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B84" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B85" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B86" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B87" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B88" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B89" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>175</v>
+      </c>
+      <c r="B90" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
         <v>179</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B91" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>184</v>
+      </c>
+      <c r="B92" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>186</v>
+      </c>
+      <c r="B93" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>187</v>
+      </c>
+      <c r="B94" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
audio stuff, some adjustments, cut down some crap
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842A1A0B-8F2D-4616-B509-C544F2DE5205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B0F3998-2440-4BB0-9093-1E2C4BE621DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6075" yWindow="2475" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,9 +517,6 @@
     <t>Remember that a polygon is formed by three or more straight lines that are connected in a loop.</t>
   </si>
   <si>
-    <t>· Round, has a center point.\n\n· Dimensions defined by two axis.</t>
-  </si>
-  <si>
     <t>tri_desc</t>
   </si>
   <si>
@@ -547,9 +544,6 @@
     <t>level_intro_4_0</t>
   </si>
   <si>
-    <t>· Formed by three or more straight lines (sides) connected in a loop.\n\n· Points are plotted on a plane.</t>
-  </si>
-  <si>
     <t>· Formed by three straight lines connected in a loop.\n· Points are plotted on a plane.\n· Angles sum up to 180°.</t>
   </si>
   <si>
@@ -589,18 +583,12 @@
     <t>As the name suggests, it is four-sided.</t>
   </si>
   <si>
-    <t>For this level, we'll be looking at three particular sub-categories that all have two pairs of opposite, parallel, equal-length sides.</t>
-  </si>
-  <si>
     <t>Just like triangles, some quadrilaterals have more than one matching categories. Keep that in mind!</t>
   </si>
   <si>
     <t>level_intro_7_0</t>
   </si>
   <si>
-    <t>Here on this level, we'll be looking at some more interesting quadrilaterals. These ones have emphasis on opposite sides and angles.</t>
-  </si>
-  <si>
     <t>level_intro_8_0</t>
   </si>
   <si>
@@ -610,9 +598,6 @@
     <t>level_intro_8_2</t>
   </si>
   <si>
-    <t>One helpful tip is look at these categories in a hierarchy. Going from top to bottom, each level shares attributes from everything above.</t>
-  </si>
-  <si>
     <t>On this final level, many of the quads will match with a bunch of categories.</t>
   </si>
   <si>
@@ -638,6 +623,21 @@
   </si>
   <si>
     <t>Congratulations!\nYou have successfully helped the spacefaring frogs survey the planet!\nBased on the analysis of the shapes gathered, the planet is habitable!\n\nThank you for playing!</t>
+  </si>
+  <si>
+    <t>· Has a center point.\n\n· Roundness defined by two axis.</t>
+  </si>
+  <si>
+    <t>· Formed by three or more straight lines (sides) connected in a loop, points are plotted on a plane.</t>
+  </si>
+  <si>
+    <t>We'll be looking at three particular quadrilaterals that have two pairs of opposite sides that are parallel, and equal-length.</t>
+  </si>
+  <si>
+    <t>On this level, we'll be looking at some more interesting quadrilaterals. These ones have emphasis on opposite sides and angles.</t>
+  </si>
+  <si>
+    <t>One helpful tip is to look at these categories in a hierarchy. Going from top to bottom, each level shares attributes from everything above.</t>
   </si>
 </sst>
 </file>
@@ -975,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,10 +1145,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1671,7 +1671,7 @@
         <v>136</v>
       </c>
       <c r="B69" t="s">
-        <v>165</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1687,23 +1687,23 @@
         <v>138</v>
       </c>
       <c r="B71" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B72" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B73" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>145</v>
       </c>
       <c r="B79" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1812,130 +1812,130 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B87" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B88" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B89" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B90" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B91" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>176</v>
+      </c>
+      <c r="B92" t="s">
         <v>178</v>
-      </c>
-      <c r="B92" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B94" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B95" t="s">
-        <v>189</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>185</v>
+      </c>
+      <c r="B96" t="s">
         <v>187</v>
-      </c>
-      <c r="B96" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B97" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B98" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B99" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B100" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B101" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding stuff to end for review, show category info when clicking on answers
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FB7C85-10BE-4CAF-A242-99DF68EEDC1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6418E7-3DE4-404E-911D-C70F2F2D7ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="2475" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9135" yWindow="2805" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="en" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
   <si>
     <t>Key</t>
   </si>
@@ -638,6 +638,54 @@
   </si>
   <si>
     <t>Just like triangles, some quadrilaterals have more than one matching category. Keep that in mind!</t>
+  </si>
+  <si>
+    <t>level_title_0</t>
+  </si>
+  <si>
+    <t>level_title_1</t>
+  </si>
+  <si>
+    <t>level_title_2</t>
+  </si>
+  <si>
+    <t>level_title_3</t>
+  </si>
+  <si>
+    <t>level_title_4</t>
+  </si>
+  <si>
+    <t>level_title_5</t>
+  </si>
+  <si>
+    <t>level_title_6</t>
+  </si>
+  <si>
+    <t>level_title_7</t>
+  </si>
+  <si>
+    <t>1 - Polygons #1</t>
+  </si>
+  <si>
+    <t>2 - Polygons #2</t>
+  </si>
+  <si>
+    <t>3 - Triangles (Angles)</t>
+  </si>
+  <si>
+    <t>4 - Triangles (Sides)</t>
+  </si>
+  <si>
+    <t>6 - Quads (Parallelograms)</t>
+  </si>
+  <si>
+    <t>7 - Quads (Misc.)</t>
+  </si>
+  <si>
+    <t>5 - Triangles (All)</t>
+  </si>
+  <si>
+    <t>8 - Quads (Hierarchy)</t>
   </si>
 </sst>
 </file>
@@ -973,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,6 +1986,70 @@
         <v>199</v>
       </c>
     </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>206</v>
+      </c>
+      <c r="B103" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>207</v>
+      </c>
+      <c r="B104" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>208</v>
+      </c>
+      <c r="B105" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>209</v>
+      </c>
+      <c r="B106" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>210</v>
+      </c>
+      <c r="B107" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>211</v>
+      </c>
+      <c r="B108" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>212</v>
+      </c>
+      <c r="B109" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>213</v>
+      </c>
+      <c r="B110" t="s">
+        <v>221</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
more update stuff based on review
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6418E7-3DE4-404E-911D-C70F2F2D7ADA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0FA4D2-B196-444A-AD52-ABDD999D2995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9135" yWindow="2805" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="228">
   <si>
     <t>Key</t>
   </si>
@@ -670,22 +670,40 @@
     <t>2 - Polygons #2</t>
   </si>
   <si>
-    <t>3 - Triangles (Angles)</t>
-  </si>
-  <si>
-    <t>4 - Triangles (Sides)</t>
-  </si>
-  <si>
-    <t>6 - Quads (Parallelograms)</t>
-  </si>
-  <si>
-    <t>7 - Quads (Misc.)</t>
-  </si>
-  <si>
-    <t>5 - Triangles (All)</t>
-  </si>
-  <si>
-    <t>8 - Quads (Hierarchy)</t>
+    <t>instruct_category_detail</t>
+  </si>
+  <si>
+    <t>Press any of the categories to review them.</t>
+  </si>
+  <si>
+    <t>level_title_8</t>
+  </si>
+  <si>
+    <t>3 - Polygons #3</t>
+  </si>
+  <si>
+    <t>4 - Triangles (Angles)</t>
+  </si>
+  <si>
+    <t>5 - Triangles (Sides)</t>
+  </si>
+  <si>
+    <t>6 - Triangles (All)</t>
+  </si>
+  <si>
+    <t>7 - Quads (Parallelograms)</t>
+  </si>
+  <si>
+    <t>8 - Quads (Types)</t>
+  </si>
+  <si>
+    <t>9 - Quads (Hierarchy)</t>
+  </si>
+  <si>
+    <t>hierarchy</t>
+  </si>
+  <si>
+    <t>Hierarchy</t>
   </si>
 </sst>
 </file>
@@ -1021,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D110"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,282 +1790,306 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>157</v>
+        <v>226</v>
       </c>
       <c r="B76" t="s">
-        <v>158</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B77" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="B78" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>145</v>
+        <v>216</v>
       </c>
       <c r="B79" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B81" t="s">
-        <v>155</v>
+        <v>198</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B82" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B84" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B85" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B86" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B87" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B88" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B89" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B90" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B91" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B92" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B93" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B94" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B95" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B96" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B97" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B98" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B99" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B100" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B101" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>195</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
+      </c>
+      <c r="B102" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>206</v>
+        <v>193</v>
       </c>
       <c r="B103" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>207</v>
-      </c>
-      <c r="B104" t="s">
-        <v>215</v>
+        <v>195</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B105" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B106" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B107" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B108" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B109" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>211</v>
+      </c>
+      <c r="B110" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>212</v>
+      </c>
+      <c r="B111" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>213</v>
       </c>
-      <c r="B110" t="s">
-        <v>221</v>
+      <c r="B112" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>218</v>
+      </c>
+      <c r="B113" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some tweaks, new build
</commit_message>
<xml_diff>
--- a/Language/language.xlsx
+++ b/Language/language.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0FA4D2-B196-444A-AD52-ABDD999D2995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E3F5CE-C109-4C58-A79F-E19302D2D60E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9135" yWindow="2805" windowWidth="19215" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,12 +553,6 @@
     <t>level_intro_5_0</t>
   </si>
   <si>
-    <t>Now that we've seen some triangles based on their angle values, let's take a look at the ones based on their side values.</t>
-  </si>
-  <si>
-    <t>For this level, we will be categorizing triangles based on their angles, and side lengths. These triangles will have more than one category that fit their attributes.</t>
-  </si>
-  <si>
     <t>quad_desc</t>
   </si>
   <si>
@@ -616,18 +610,9 @@
     <t>Final Score:</t>
   </si>
   <si>
-    <t>In this game, you will be helping these fine capable frogs analyze a potentially habitable planet by identifying the shapes scattered across the land.</t>
-  </si>
-  <si>
     <t>Congratulations!\nYou have successfully helped the spacefaring frogs survey the planet!\nBased on the analysis of the shapes gathered, the planet is habitable!\n\nThank you for playing!</t>
   </si>
   <si>
-    <t>· Has a center point.\n\n· Roundness defined by two axis.</t>
-  </si>
-  <si>
-    <t>· Formed by three or more straight lines (sides) connected in a loop, points are plotted on a plane.</t>
-  </si>
-  <si>
     <t>We'll be looking at three particular quadrilaterals that have two pairs of opposite sides that are parallel, and equal-length.</t>
   </si>
   <si>
@@ -704,6 +689,21 @@
   </si>
   <si>
     <t>Hierarchy</t>
+  </si>
+  <si>
+    <t>In this game, you will be helping these fine and capable frogs to analyze a potentially habitable planet by identifying the shapes scattered across the land.</t>
+  </si>
+  <si>
+    <t>· Has a center point.\n\n· Roundness defined by two axes.</t>
+  </si>
+  <si>
+    <t>· Formed by three or more straight lines (sides) connected in a loop. Points are plotted on a plane.</t>
+  </si>
+  <si>
+    <t>Now that we've seen some triangles based on their angle values, let's take a look at some more based on their side values.</t>
+  </si>
+  <si>
+    <t>For this level, we will be categorizing triangles based on their angles AND side lengths. These triangles will have more than one category that fit their attributes.</t>
   </si>
 </sst>
 </file>
@@ -1041,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,10 +1211,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1737,7 +1737,7 @@
         <v>136</v>
       </c>
       <c r="B69" t="s">
-        <v>200</v>
+        <v>224</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -1753,7 +1753,7 @@
         <v>138</v>
       </c>
       <c r="B71" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -1766,10 +1766,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B73" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -1790,10 +1790,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B76" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -1814,10 +1814,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B79" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -1833,7 +1833,7 @@
         <v>145</v>
       </c>
       <c r="B81" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -1929,7 +1929,7 @@
         <v>173</v>
       </c>
       <c r="B93" t="s">
-        <v>177</v>
+        <v>226</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -1937,159 +1937,159 @@
         <v>176</v>
       </c>
       <c r="B94" t="s">
-        <v>178</v>
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B95" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B96" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B97" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B98" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B99" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B100" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B101" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>188</v>
+      </c>
+      <c r="B102" t="s">
         <v>190</v>
-      </c>
-      <c r="B102" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B103" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B105" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B106" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B107" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B108" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B109" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B110" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B111" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B112" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B113" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>